<commit_message>
covid daily emissions update
</commit_message>
<xml_diff>
--- a/Results/Plot data/ipcc_ar6_figure_spm1_gases.xlsx
+++ b/Results/Plot data/ipcc_ar6_figure_spm1_gases.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="60">
   <si>
     <t>Author</t>
   </si>
@@ -196,6 +196,12 @@
   </si>
   <si>
     <t>low</t>
+  </si>
+  <si>
+    <t>abs growth since 1990</t>
+  </si>
+  <si>
+    <t>share of gas in total</t>
   </si>
 </sst>
 </file>
@@ -203,7 +209,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -245,7 +251,7 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
@@ -583,11 +589,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH18"/>
+  <dimension ref="A1:AH30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Y12" sqref="Y12"/>
+      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AH8" sqref="AH8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1346,6 +1352,10 @@
         <v>6.2589216416476345</v>
       </c>
       <c r="AG8" s="2"/>
+      <c r="AH8" s="2">
+        <f>AE5-AD5</f>
+        <v>0.91477574890132995</v>
+      </c>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
@@ -1473,123 +1483,172 @@
       <c r="AE10" s="2"/>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="AE11" s="3"/>
+      <c r="V11" s="3">
+        <f t="shared" ref="V11:AD11" si="6">SUM(V5:V6)</f>
+        <v>39.474271411270074</v>
+      </c>
+      <c r="W11" s="3">
+        <f t="shared" si="6"/>
+        <v>40.203218775721069</v>
+      </c>
+      <c r="X11" s="3">
+        <f t="shared" si="6"/>
+        <v>41.1137936286121</v>
+      </c>
+      <c r="Y11" s="3">
+        <f t="shared" si="6"/>
+        <v>41.746130115096427</v>
+      </c>
+      <c r="Z11" s="3">
+        <f t="shared" si="6"/>
+        <v>42.377909286418074</v>
+      </c>
+      <c r="AA11" s="3">
+        <f t="shared" si="6"/>
+        <v>42.625562341542299</v>
+      </c>
+      <c r="AB11" s="3">
+        <f t="shared" si="6"/>
+        <v>42.119950820300168</v>
+      </c>
+      <c r="AC11" s="3">
+        <f t="shared" si="6"/>
+        <v>42.510330716421699</v>
+      </c>
+      <c r="AD11" s="3">
+        <f t="shared" si="6"/>
+        <v>43.336479134442371</v>
+      </c>
+      <c r="AE11" s="3">
+        <f>SUM(AE5:AE6)</f>
+        <v>44.535093622877099</v>
+      </c>
+      <c r="AF11" s="1">
+        <f>((AE11/V11)^(AE1-V1))-1</f>
+        <v>1.9613805598825484</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AF12" s="1">
+        <f>((AD11/V11)^(AD1-V1))-1</f>
+        <v>1.1101630353862135</v>
+      </c>
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B14">
-        <f>(B2*$AH2)^2</f>
+        <f t="shared" ref="B14:AE14" si="7">(B2*$AH2)^2</f>
         <v>7.3842844940552339E-3</v>
       </c>
       <c r="C14">
-        <f>(C2*$AH2)^2</f>
+        <f t="shared" si="7"/>
         <v>8.6138428815969396E-3</v>
       </c>
       <c r="D14">
-        <f>(D2*$AH2)^2</f>
+        <f t="shared" si="7"/>
         <v>8.8212758499851013E-3</v>
       </c>
       <c r="E14">
-        <f>(E2*$AH2)^2</f>
+        <f t="shared" si="7"/>
         <v>1.0295605565509949E-2</v>
       </c>
       <c r="F14">
-        <f>(F2*$AH2)^2</f>
+        <f t="shared" si="7"/>
         <v>1.2385391619835734E-2</v>
       </c>
       <c r="G14">
-        <f>(G2*$AH2)^2</f>
+        <f t="shared" si="7"/>
         <v>1.5126148789623263E-2</v>
       </c>
       <c r="H14">
-        <f>(H2*$AH2)^2</f>
+        <f t="shared" si="7"/>
         <v>1.7398224118794912E-2</v>
       </c>
       <c r="I14">
-        <f>(I2*$AH2)^2</f>
+        <f t="shared" si="7"/>
         <v>1.9615213855290314E-2</v>
       </c>
       <c r="J14">
-        <f>(J2*$AH2)^2</f>
+        <f t="shared" si="7"/>
         <v>2.1409198501415261E-2</v>
       </c>
       <c r="K14">
-        <f>(K2*$AH2)^2</f>
+        <f t="shared" si="7"/>
         <v>2.3432184402496049E-2</v>
       </c>
       <c r="L14">
-        <f>(L2*$AH2)^2</f>
+        <f t="shared" si="7"/>
         <v>2.4760951116004504E-2</v>
       </c>
       <c r="M14">
-        <f>(M2*$AH2)^2</f>
+        <f t="shared" si="7"/>
         <v>2.4047619139166216E-2</v>
       </c>
       <c r="N14">
-        <f>(N2*$AH2)^2</f>
+        <f t="shared" si="7"/>
         <v>2.4622159593279947E-2</v>
       </c>
       <c r="O14">
-        <f>(O2*$AH2)^2</f>
+        <f t="shared" si="7"/>
         <v>2.6195969744096249E-2</v>
       </c>
       <c r="P14">
-        <f>(P2*$AH2)^2</f>
+        <f t="shared" si="7"/>
         <v>3.0845714793964966E-2</v>
       </c>
       <c r="Q14">
-        <f>(Q2*$AH2)^2</f>
+        <f t="shared" si="7"/>
         <v>3.5073529429829164E-2</v>
       </c>
       <c r="R14">
-        <f>(R2*$AH2)^2</f>
+        <f t="shared" si="7"/>
         <v>3.2321749584650741E-2</v>
       </c>
       <c r="S14">
-        <f>(S2*$AH2)^2</f>
+        <f t="shared" si="7"/>
         <v>3.449649928384222E-2</v>
       </c>
       <c r="T14">
-        <f>(T2*$AH2)^2</f>
+        <f t="shared" si="7"/>
         <v>3.1144906385482025E-2</v>
       </c>
       <c r="U14">
-        <f>(U2*$AH2)^2</f>
+        <f t="shared" si="7"/>
         <v>3.3229736464819581E-2</v>
       </c>
       <c r="V14">
-        <f>(V2*$AH2)^2</f>
+        <f t="shared" si="7"/>
         <v>3.8916079885414345E-2</v>
       </c>
       <c r="W14">
-        <f>(W2*$AH2)^2</f>
+        <f t="shared" si="7"/>
         <v>4.258549366767788E-2</v>
       </c>
       <c r="X14">
-        <f>(X2*$AH2)^2</f>
+        <f t="shared" si="7"/>
         <v>4.508524993012266E-2</v>
       </c>
       <c r="Y14">
-        <f>(Y2*$AH2)^2</f>
+        <f t="shared" si="7"/>
         <v>4.423180230492272E-2</v>
       </c>
       <c r="Z14">
-        <f>(Z2*$AH2)^2</f>
+        <f t="shared" si="7"/>
         <v>4.7058437770085386E-2</v>
       </c>
       <c r="AA14">
-        <f>(AA2*$AH2)^2</f>
+        <f t="shared" si="7"/>
         <v>4.2783728240271469E-2</v>
       </c>
       <c r="AB14">
-        <f>(AB2*$AH2)^2</f>
+        <f t="shared" si="7"/>
         <v>4.3201738658049764E-2</v>
       </c>
       <c r="AC14">
-        <f>(AC2*$AH2)^2</f>
+        <f t="shared" si="7"/>
         <v>4.3421898486838716E-2</v>
       </c>
       <c r="AD14">
-        <f>(AD2*$AH2)^2</f>
+        <f t="shared" si="7"/>
         <v>4.3231110396986662E-2</v>
       </c>
       <c r="AE14">
@@ -1599,490 +1658,540 @@
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B15">
-        <f>(B3*$AH3)^2</f>
+        <f t="shared" ref="B15:AE15" si="8">(B3*$AH3)^2</f>
         <v>1.2972310572723731</v>
       </c>
       <c r="C15">
-        <f>(C3*$AH3)^2</f>
+        <f t="shared" si="8"/>
         <v>1.2847499074026159</v>
       </c>
       <c r="D15">
-        <f>(D3*$AH3)^2</f>
+        <f t="shared" si="8"/>
         <v>1.3037364653351136</v>
       </c>
       <c r="E15">
-        <f>(E3*$AH3)^2</f>
+        <f t="shared" si="8"/>
         <v>1.3160856983196656</v>
       </c>
       <c r="F15">
-        <f>(F3*$AH3)^2</f>
+        <f t="shared" si="8"/>
         <v>1.3690752580969603</v>
       </c>
       <c r="G15">
-        <f>(G3*$AH3)^2</f>
+        <f t="shared" si="8"/>
         <v>1.4223809965243681</v>
       </c>
       <c r="H15">
-        <f>(H3*$AH3)^2</f>
+        <f t="shared" si="8"/>
         <v>1.4793294235715417</v>
       </c>
       <c r="I15">
-        <f>(I3*$AH3)^2</f>
+        <f t="shared" si="8"/>
         <v>1.4827056002409866</v>
       </c>
       <c r="J15">
-        <f>(J3*$AH3)^2</f>
+        <f t="shared" si="8"/>
         <v>1.458369898353477</v>
       </c>
       <c r="K15">
-        <f>(K3*$AH3)^2</f>
+        <f t="shared" si="8"/>
         <v>1.458823034798794</v>
       </c>
       <c r="L15">
-        <f>(L3*$AH3)^2</f>
+        <f t="shared" si="8"/>
         <v>1.4923814933583313</v>
       </c>
       <c r="M15">
-        <f>(M3*$AH3)^2</f>
+        <f t="shared" si="8"/>
         <v>1.5040894935735245</v>
       </c>
       <c r="N15">
-        <f>(N3*$AH3)^2</f>
+        <f t="shared" si="8"/>
         <v>1.5133281531229794</v>
       </c>
       <c r="O15">
-        <f>(O3*$AH3)^2</f>
+        <f t="shared" si="8"/>
         <v>1.5683114160251199</v>
       </c>
       <c r="P15">
-        <f>(P3*$AH3)^2</f>
+        <f t="shared" si="8"/>
         <v>1.6610084557429659</v>
       </c>
       <c r="Q15">
-        <f>(Q3*$AH3)^2</f>
+        <f t="shared" si="8"/>
         <v>1.6989925044379814</v>
       </c>
       <c r="R15">
-        <f>(R3*$AH3)^2</f>
+        <f t="shared" si="8"/>
         <v>1.7411420762229304</v>
       </c>
       <c r="S15">
-        <f>(S3*$AH3)^2</f>
+        <f t="shared" si="8"/>
         <v>1.8259741498873787</v>
       </c>
       <c r="T15">
-        <f>(T3*$AH3)^2</f>
+        <f t="shared" si="8"/>
         <v>1.8034065318864363</v>
       </c>
       <c r="U15">
-        <f>(U3*$AH3)^2</f>
+        <f t="shared" si="8"/>
         <v>1.7871024075088719</v>
       </c>
       <c r="V15">
-        <f>(V3*$AH3)^2</f>
+        <f t="shared" si="8"/>
         <v>1.8564955458705226</v>
       </c>
       <c r="W15">
-        <f>(W3*$AH3)^2</f>
+        <f t="shared" si="8"/>
         <v>1.9384799531141821</v>
       </c>
       <c r="X15">
-        <f>(X3*$AH3)^2</f>
+        <f t="shared" si="8"/>
         <v>1.9798767203438745</v>
       </c>
       <c r="Y15">
-        <f>(Y3*$AH3)^2</f>
+        <f t="shared" si="8"/>
         <v>2.0504252585162175</v>
       </c>
       <c r="Z15">
-        <f>(Z3*$AH3)^2</f>
+        <f t="shared" si="8"/>
         <v>2.0954158540667382</v>
       </c>
       <c r="AA15">
-        <f>(AA3*$AH3)^2</f>
+        <f t="shared" si="8"/>
         <v>2.122431503923226</v>
       </c>
       <c r="AB15">
-        <f>(AB3*$AH3)^2</f>
+        <f t="shared" si="8"/>
         <v>2.1950863472034867</v>
       </c>
       <c r="AC15">
-        <f>(AC3*$AH3)^2</f>
+        <f t="shared" si="8"/>
         <v>2.235384656776044</v>
       </c>
       <c r="AD15">
-        <f>(AD3*$AH3)^2</f>
+        <f t="shared" si="8"/>
         <v>2.2517733345302204</v>
       </c>
       <c r="AE15">
-        <f>(AE3*$AH3)^2</f>
+        <f t="shared" si="8"/>
         <v>2.3092043479634388</v>
       </c>
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B16">
-        <f>(B4*$AH4)^2</f>
+        <f t="shared" ref="B16:AE16" si="9">(B4*$AH4)^2</f>
         <v>6.0156137088173764</v>
       </c>
       <c r="C16">
-        <f>(C4*$AH4)^2</f>
+        <f t="shared" si="9"/>
         <v>5.9350818325181489</v>
       </c>
       <c r="D16">
-        <f>(D4*$AH4)^2</f>
+        <f t="shared" si="9"/>
         <v>5.9387438803530861</v>
       </c>
       <c r="E16">
-        <f>(E4*$AH4)^2</f>
+        <f t="shared" si="9"/>
         <v>5.9212974292457048</v>
       </c>
       <c r="F16">
-        <f>(F4*$AH4)^2</f>
+        <f t="shared" si="9"/>
         <v>6.0046214813893259</v>
       </c>
       <c r="G16">
-        <f>(G4*$AH4)^2</f>
+        <f t="shared" si="9"/>
         <v>6.1712736923419991</v>
       </c>
       <c r="H16">
-        <f>(H4*$AH4)^2</f>
+        <f t="shared" si="9"/>
         <v>6.3179614087918168</v>
       </c>
       <c r="I16">
-        <f>(I4*$AH4)^2</f>
+        <f t="shared" si="9"/>
         <v>6.3089157443963586</v>
       </c>
       <c r="J16">
-        <f>(J4*$AH4)^2</f>
+        <f t="shared" si="9"/>
         <v>6.1715917951450701</v>
       </c>
       <c r="K16">
-        <f>(K4*$AH4)^2</f>
+        <f t="shared" si="9"/>
         <v>6.2201637683559818</v>
       </c>
       <c r="L16">
-        <f>(L4*$AH4)^2</f>
+        <f t="shared" si="9"/>
         <v>6.4075127266302143</v>
       </c>
       <c r="M16">
-        <f>(M4*$AH4)^2</f>
+        <f t="shared" si="9"/>
         <v>6.4285830019317425</v>
       </c>
       <c r="N16">
-        <f>(N4*$AH4)^2</f>
+        <f t="shared" si="9"/>
         <v>6.4229585066811286</v>
       </c>
       <c r="O16">
-        <f>(O4*$AH4)^2</f>
+        <f t="shared" si="9"/>
         <v>6.8310477152766644</v>
       </c>
       <c r="P16">
-        <f>(P4*$AH4)^2</f>
+        <f t="shared" si="9"/>
         <v>7.1457997010565384</v>
       </c>
       <c r="Q16">
-        <f>(Q4*$AH4)^2</f>
+        <f t="shared" si="9"/>
         <v>7.4393281445687256</v>
       </c>
       <c r="R16">
-        <f>(R4*$AH4)^2</f>
+        <f t="shared" si="9"/>
         <v>7.7323067006577562</v>
       </c>
       <c r="S16">
-        <f>(S4*$AH4)^2</f>
+        <f t="shared" si="9"/>
         <v>7.8759126333913034</v>
       </c>
       <c r="T16">
-        <f>(T4*$AH4)^2</f>
+        <f t="shared" si="9"/>
         <v>8.1490384897453971</v>
       </c>
       <c r="U16">
-        <f>(U4*$AH4)^2</f>
+        <f t="shared" si="9"/>
         <v>8.1099733548725492</v>
       </c>
       <c r="V16">
-        <f>(V4*$AH4)^2</f>
+        <f t="shared" si="9"/>
         <v>8.4057942822976806</v>
       </c>
       <c r="W16">
-        <f>(W4*$AH4)^2</f>
+        <f t="shared" si="9"/>
         <v>8.7566021705291686</v>
       </c>
       <c r="X16">
-        <f>(X4*$AH4)^2</f>
+        <f t="shared" si="9"/>
         <v>8.9984881337454219</v>
       </c>
       <c r="Y16">
-        <f>(Y4*$AH4)^2</f>
+        <f t="shared" si="9"/>
         <v>9.1006065830399159</v>
       </c>
       <c r="Z16">
-        <f>(Z4*$AH4)^2</f>
+        <f t="shared" si="9"/>
         <v>9.2481004076152526</v>
       </c>
       <c r="AA16">
-        <f>(AA4*$AH4)^2</f>
+        <f t="shared" si="9"/>
         <v>9.3449665248811229</v>
       </c>
       <c r="AB16">
-        <f>(AB4*$AH4)^2</f>
+        <f t="shared" si="9"/>
         <v>9.4226378600181508</v>
       </c>
       <c r="AC16">
-        <f>(AC4*$AH4)^2</f>
+        <f t="shared" si="9"/>
         <v>9.684426974233169</v>
       </c>
       <c r="AD16">
-        <f>(AD4*$AH4)^2</f>
+        <f t="shared" si="9"/>
         <v>9.8374608934389514</v>
       </c>
       <c r="AE16">
-        <f>(AE4*$AH4)^2</f>
+        <f t="shared" si="9"/>
         <v>10.047431494399873</v>
       </c>
     </row>
-    <row r="17" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B17">
-        <f>(B5*$AH5)^2</f>
+        <f t="shared" ref="B17:AE17" si="10">(B5*$AH5)^2</f>
         <v>12.14819834286296</v>
       </c>
       <c r="C17">
-        <f>(C5*$AH5)^2</f>
+        <f t="shared" si="10"/>
         <v>11.943528051264105</v>
       </c>
       <c r="D17">
-        <f>(D5*$AH5)^2</f>
+        <f t="shared" si="10"/>
         <v>11.980837482960359</v>
       </c>
       <c r="E17">
-        <f>(E5*$AH5)^2</f>
+        <f t="shared" si="10"/>
         <v>12.008102901786271</v>
       </c>
       <c r="F17">
-        <f>(F5*$AH5)^2</f>
+        <f t="shared" si="10"/>
         <v>11.895948386485721</v>
       </c>
       <c r="G17">
-        <f>(G5*$AH5)^2</f>
+        <f t="shared" si="10"/>
         <v>11.7259082452287</v>
       </c>
       <c r="H17">
-        <f>(H5*$AH5)^2</f>
+        <f t="shared" si="10"/>
         <v>11.43031036681724</v>
       </c>
       <c r="I17">
-        <f>(I5*$AH5)^2</f>
+        <f t="shared" si="10"/>
         <v>21.044106310598515</v>
       </c>
       <c r="J17">
-        <f>(J5*$AH5)^2</f>
+        <f t="shared" si="10"/>
         <v>10.220027590187003</v>
       </c>
       <c r="K17">
-        <f>(K5*$AH5)^2</f>
+        <f t="shared" si="10"/>
         <v>9.9608245977033132</v>
       </c>
       <c r="L17">
-        <f>(L5*$AH5)^2</f>
+        <f t="shared" si="10"/>
         <v>12.504659446109223</v>
       </c>
       <c r="M17">
-        <f>(M5*$AH5)^2</f>
+        <f t="shared" si="10"/>
         <v>11.697373873387793</v>
       </c>
       <c r="N17">
-        <f>(N5*$AH5)^2</f>
+        <f t="shared" si="10"/>
         <v>14.824785818462081</v>
       </c>
       <c r="O17">
-        <f>(O5*$AH5)^2</f>
+        <f t="shared" si="10"/>
         <v>15.726129119639477</v>
       </c>
       <c r="P17">
-        <f>(P5*$AH5)^2</f>
+        <f t="shared" si="10"/>
         <v>15.076103768416226</v>
       </c>
       <c r="Q17">
-        <f>(Q5*$AH5)^2</f>
+        <f t="shared" si="10"/>
         <v>13.220745479900764</v>
       </c>
       <c r="R17">
-        <f>(R5*$AH5)^2</f>
+        <f t="shared" si="10"/>
         <v>14.722019468359068</v>
       </c>
       <c r="S17">
-        <f>(S5*$AH5)^2</f>
+        <f t="shared" si="10"/>
         <v>11.318612258010763</v>
       </c>
       <c r="T17">
-        <f>(T5*$AH5)^2</f>
+        <f t="shared" si="10"/>
         <v>12.128578030031662</v>
       </c>
       <c r="U17">
-        <f>(U5*$AH5)^2</f>
+        <f t="shared" si="10"/>
         <v>16.861778542400927</v>
       </c>
       <c r="V17">
-        <f>(V5*$AH5)^2</f>
+        <f t="shared" si="10"/>
         <v>13.958606136926562</v>
       </c>
       <c r="W17">
-        <f>(W5*$AH5)^2</f>
+        <f t="shared" si="10"/>
         <v>12.556084245819125</v>
       </c>
       <c r="X17">
-        <f>(X5*$AH5)^2</f>
+        <f t="shared" si="10"/>
         <v>14.526947627301601</v>
       </c>
       <c r="Y17">
-        <f>(Y5*$AH5)^2</f>
+        <f t="shared" si="10"/>
         <v>15.476729139182313</v>
       </c>
       <c r="Z17">
-        <f>(Z5*$AH5)^2</f>
+        <f t="shared" si="10"/>
         <v>17.894330050021804</v>
       </c>
       <c r="AA17">
-        <f>(AA5*$AH5)^2</f>
+        <f t="shared" si="10"/>
         <v>19.131116356764831</v>
       </c>
       <c r="AB17">
-        <f>(AB5*$AH5)^2</f>
+        <f t="shared" si="10"/>
         <v>15.913247507290993</v>
       </c>
       <c r="AC17">
-        <f>(AC5*$AH5)^2</f>
+        <f t="shared" si="10"/>
         <v>15.223996833874054</v>
       </c>
       <c r="AD17">
-        <f>(AD5*$AH5)^2</f>
+        <f t="shared" si="10"/>
         <v>15.865756124881777</v>
       </c>
       <c r="AE17">
-        <f>(AE5*$AH5)^2</f>
+        <f t="shared" si="10"/>
         <v>21.377003707369518</v>
       </c>
     </row>
-    <row r="18" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B18">
-        <f>(B6*$AH6)^2</f>
+        <f t="shared" ref="B18:AE18" si="11">(B6*$AH6)^2</f>
         <v>3.2992792030164773</v>
       </c>
       <c r="C18">
-        <f>(C6*$AH6)^2</f>
+        <f t="shared" si="11"/>
         <v>3.3379421061232373</v>
       </c>
       <c r="D18">
-        <f>(D6*$AH6)^2</f>
+        <f t="shared" si="11"/>
         <v>3.3189984526045051</v>
       </c>
       <c r="E18">
-        <f>(E6*$AH6)^2</f>
+        <f t="shared" si="11"/>
         <v>3.3477806272156179</v>
       </c>
       <c r="F18">
-        <f>(F6*$AH6)^2</f>
+        <f t="shared" si="11"/>
         <v>3.4177995024247285</v>
       </c>
       <c r="G18">
-        <f>(G6*$AH6)^2</f>
+        <f t="shared" si="11"/>
         <v>3.6140663339241761</v>
       </c>
       <c r="H18">
-        <f>(H6*$AH6)^2</f>
+        <f t="shared" si="11"/>
         <v>3.7508273803854091</v>
       </c>
       <c r="I18">
-        <f>(I6*$AH6)^2</f>
+        <f t="shared" si="11"/>
         <v>3.8916584299309371</v>
       </c>
       <c r="J18">
-        <f>(J6*$AH6)^2</f>
+        <f t="shared" si="11"/>
         <v>3.9391534325950657</v>
       </c>
       <c r="K18">
-        <f>(K6*$AH6)^2</f>
+        <f t="shared" si="11"/>
         <v>3.989314091182838</v>
       </c>
       <c r="L18">
-        <f>(L6*$AH6)^2</f>
+        <f t="shared" si="11"/>
         <v>4.2641867240407016</v>
       </c>
       <c r="M18">
-        <f>(M6*$AH6)^2</f>
+        <f t="shared" si="11"/>
         <v>4.372062156604744</v>
       </c>
       <c r="N18">
-        <f>(N6*$AH6)^2</f>
+        <f t="shared" si="11"/>
         <v>4.4937053948171197</v>
       </c>
       <c r="O18">
-        <f>(O6*$AH6)^2</f>
+        <f t="shared" si="11"/>
         <v>4.9328156857720833</v>
       </c>
       <c r="P18">
-        <f>(P6*$AH6)^2</f>
+        <f t="shared" si="11"/>
         <v>5.4021108947918925</v>
       </c>
       <c r="Q18">
-        <f>(Q6*$AH6)^2</f>
+        <f t="shared" si="11"/>
         <v>5.8116885058146339</v>
       </c>
       <c r="R18">
-        <f>(R6*$AH6)^2</f>
+        <f t="shared" si="11"/>
         <v>6.2153261282221548</v>
       </c>
       <c r="S18">
-        <f>(S6*$AH6)^2</f>
+        <f t="shared" si="11"/>
         <v>6.7038906656976378</v>
       </c>
       <c r="T18">
-        <f>(T6*$AH6)^2</f>
+        <f t="shared" si="11"/>
         <v>6.7939379522473455</v>
       </c>
       <c r="U18">
-        <f>(U6*$AH6)^2</f>
+        <f t="shared" si="11"/>
         <v>6.6514353523155316</v>
       </c>
       <c r="V18">
-        <f>(V6*$AH6)^2</f>
+        <f t="shared" si="11"/>
         <v>7.4581226611612301</v>
       </c>
       <c r="W18">
-        <f>(W6*$AH6)^2</f>
+        <f t="shared" si="11"/>
         <v>7.9033573139729354</v>
       </c>
       <c r="X18">
-        <f>(X6*$AH6)^2</f>
+        <f t="shared" si="11"/>
         <v>8.1425321904104457</v>
       </c>
       <c r="Y18">
-        <f>(Y6*$AH6)^2</f>
+        <f t="shared" si="11"/>
         <v>8.3525912450928441</v>
       </c>
       <c r="Z18">
-        <f>(Z6*$AH6)^2</f>
+        <f t="shared" si="11"/>
         <v>8.449398183938639</v>
       </c>
       <c r="AA18">
-        <f>(AA6*$AH6)^2</f>
+        <f t="shared" si="11"/>
         <v>8.4690847567704512</v>
       </c>
       <c r="AB18">
-        <f>(AB6*$AH6)^2</f>
+        <f t="shared" si="11"/>
         <v>8.4896139743574182</v>
       </c>
       <c r="AC18">
-        <f>(AC6*$AH6)^2</f>
+        <f t="shared" si="11"/>
         <v>8.7314761879615013</v>
       </c>
       <c r="AD18">
-        <f>(AD6*$AH6)^2</f>
+        <f t="shared" si="11"/>
         <v>9.0703205235832716</v>
       </c>
       <c r="AE18">
-        <f>(AE6*$AH6)^2</f>
+        <f t="shared" si="11"/>
         <v>9.2076099536353357</v>
+      </c>
+      <c r="AF18">
+        <f>SQRT(SUM(V17:V18))</f>
+        <v>4.6278211717921636</v>
+      </c>
+    </row>
+    <row r="21" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="AE21" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="AE22" s="4">
+        <f>(AE2-B2)/B2</f>
+        <v>1.4166927350799441</v>
+      </c>
+    </row>
+    <row r="23" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="AE23" s="4">
+        <f t="shared" ref="AE23:AE28" si="12">(AE3-B3)/B3</f>
+        <v>0.3342048481999545</v>
+      </c>
+    </row>
+    <row r="24" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="AE24" s="4">
+        <f t="shared" si="12"/>
+        <v>0.29237204908754477</v>
+      </c>
+    </row>
+    <row r="25" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="AE25" s="4">
+        <f t="shared" si="12"/>
+        <v>0.32653123127173178</v>
+      </c>
+    </row>
+    <row r="26" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="AE26" s="4">
+        <f t="shared" si="12"/>
+        <v>0.67056709204942899</v>
+      </c>
+    </row>
+    <row r="28" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="AE28" s="4">
+        <f t="shared" si="12"/>
+        <v>0.53310213997777989</v>
+      </c>
+    </row>
+    <row r="30" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="AE30" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
edgar6_v5 update N2O emissions all figures
</commit_message>
<xml_diff>
--- a/Results/Plot data/ipcc_ar6_figure_spm1_gases.xlsx
+++ b/Results/Plot data/ipcc_ar6_figure_spm1_gases.xlsx
@@ -12,12 +12,13 @@
     <sheet name="panel a shares" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="panel b" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="panel c" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="spm table" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
   <si>
     <t xml:space="preserve">Author</t>
   </si>
@@ -28,7 +29,7 @@
     <t xml:space="preserve">Last update</t>
   </si>
   <si>
-    <t xml:space="preserve">2021-10-12 13:46:09</t>
+    <t xml:space="preserve">2021-10-13 15:18:12</t>
   </si>
   <si>
     <t xml:space="preserve">Code</t>
@@ -40,6 +41,9 @@
     <t xml:space="preserve">gas</t>
   </si>
   <si>
+    <t xml:space="preserve">var</t>
+  </si>
+  <si>
     <t xml:space="preserve">1990</t>
   </si>
   <si>
@@ -130,19 +134,28 @@
     <t xml:space="preserve">2019</t>
   </si>
   <si>
+    <t xml:space="preserve">CO2 FFI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CO2 LULUCF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CH4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N2O</t>
+  </si>
+  <si>
     <t xml:space="preserve">Fgas</t>
   </si>
   <si>
-    <t xml:space="preserve">N2O</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CH4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CO2 LULUCF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CO2 FFI</t>
+    <t xml:space="preserve">Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uncertainty</t>
   </si>
   <si>
     <t xml:space="preserve">year</t>
@@ -175,9 +188,6 @@
     <t xml:space="preserve">id</t>
   </si>
   <si>
-    <t xml:space="preserve">uncertainty</t>
-  </si>
-  <si>
     <t xml:space="preserve">abs_uncertainty</t>
   </si>
   <si>
@@ -206,6 +216,69 @@
   </si>
   <si>
     <t xml:space="preserve">low</t>
+  </si>
+  <si>
+    <t xml:space="preserve"/>
+  </si>
+  <si>
+    <t xml:space="preserve">2019 Emissions (GtCO2eq)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">38±3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.6±4.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11±3.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.7±1.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.4±0.41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">59±6.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1990-2019 Growth (GtCO2eq)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15±1.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.6±1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.4±0.72</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.65±0.39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.97±0.29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21±1.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1990-2019 Growth (%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 67</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 33</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">250</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 54</t>
   </si>
 </sst>
 </file>
@@ -669,480 +742,1184 @@
       <c r="AE1" t="s">
         <v>36</v>
       </c>
+      <c r="AF1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" t="n">
-        <v>0.381216423881282</v>
+        <v>38</v>
+      </c>
+      <c r="B2" t="s">
+        <v>39</v>
       </c>
       <c r="C2" t="n">
-        <v>0.396099605425283</v>
+        <v>22.7278825117111</v>
       </c>
       <c r="D2" t="n">
-        <v>0.403242312333865</v>
+        <v>22.8608054458048</v>
       </c>
       <c r="E2" t="n">
-        <v>0.415991162732946</v>
+        <v>22.7973204857492</v>
       </c>
       <c r="F2" t="n">
-        <v>0.449428755046009</v>
+        <v>22.8952027577176</v>
       </c>
       <c r="G2" t="n">
-        <v>0.498128786341533</v>
+        <v>23.1341608835042</v>
       </c>
       <c r="H2" t="n">
-        <v>0.531939552487414</v>
+        <v>23.791417902752</v>
       </c>
       <c r="I2" t="n">
-        <v>0.566835583280444</v>
+        <v>24.2389537984593</v>
       </c>
       <c r="J2" t="n">
-        <v>0.59561157093514</v>
+        <v>24.6896179009045</v>
       </c>
       <c r="K2" t="n">
-        <v>0.61777226901104</v>
+        <v>24.8245264087741</v>
       </c>
       <c r="L2" t="n">
-        <v>0.655705087850153</v>
+        <v>25.0005469983828</v>
       </c>
       <c r="M2" t="n">
-        <v>0.660155956268442</v>
+        <v>25.8473180868132</v>
       </c>
       <c r="N2" t="n">
-        <v>0.737170097917884</v>
+        <v>26.1715889388161</v>
       </c>
       <c r="O2" t="n">
-        <v>0.767393658719658</v>
+        <v>26.5344190665088</v>
       </c>
       <c r="P2" t="n">
-        <v>0.8480087680807</v>
+        <v>27.7995268106743</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.908472287744949</v>
+        <v>29.0925481751366</v>
       </c>
       <c r="R2" t="n">
-        <v>0.877785810766169</v>
+        <v>30.1700253299925</v>
       </c>
       <c r="S2" t="n">
-        <v>0.879118168819757</v>
+        <v>31.2005699011361</v>
       </c>
       <c r="T2" t="n">
-        <v>0.855568648353471</v>
+        <v>32.4060315289608</v>
       </c>
       <c r="U2" t="n">
-        <v>0.877874049586454</v>
+        <v>32.6214980936267</v>
       </c>
       <c r="V2" t="n">
-        <v>0.942758172493304</v>
+        <v>32.2803160523147</v>
       </c>
       <c r="W2" t="n">
-        <v>0.998046611981724</v>
+        <v>34.180727136629</v>
       </c>
       <c r="X2" t="n">
-        <v>1.05967117039715</v>
+        <v>35.1857131825334</v>
       </c>
       <c r="Y2" t="n">
-        <v>1.11234348344948</v>
+        <v>35.70530452658</v>
       </c>
       <c r="Z2" t="n">
-        <v>1.19209320678856</v>
+        <v>36.1708689261492</v>
       </c>
       <c r="AA2" t="n">
-        <v>1.15386683147162</v>
+        <v>36.3705476959089</v>
       </c>
       <c r="AB2" t="n">
-        <v>1.20861676001377</v>
+        <v>36.3859481897665</v>
       </c>
       <c r="AC2" t="n">
-        <v>1.27784706057641</v>
+        <v>36.4655894610653</v>
       </c>
       <c r="AD2" t="n">
-        <v>1.34470422904084</v>
+        <v>36.9355932676273</v>
       </c>
       <c r="AE2" t="n">
-        <v>1.35028402604853</v>
+        <v>37.7161806699703</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>37.9113691280531</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" t="n">
-        <v>2.00642716754084</v>
+        <v>40</v>
+      </c>
+      <c r="B3" t="s">
+        <v>39</v>
       </c>
       <c r="C3" t="n">
-        <v>1.99939597916104</v>
+        <v>4.979180807728</v>
       </c>
       <c r="D3" t="n">
-        <v>2.01570991212078</v>
+        <v>4.93705854162133</v>
       </c>
       <c r="E3" t="n">
-        <v>2.01129632106231</v>
+        <v>4.94476376996267</v>
       </c>
       <c r="F3" t="n">
-        <v>2.05574953817727</v>
+        <v>4.95038710129067</v>
       </c>
       <c r="G3" t="n">
-        <v>2.11970750819197</v>
+        <v>4.92721480013867</v>
       </c>
       <c r="H3" t="n">
-        <v>2.16758632501459</v>
+        <v>4.89187336204267</v>
       </c>
       <c r="I3" t="n">
-        <v>2.1574787499978</v>
+        <v>4.829820287952</v>
       </c>
       <c r="J3" t="n">
-        <v>2.14042841905745</v>
+        <v>6.55340794822933</v>
       </c>
       <c r="K3" t="n">
-        <v>2.14834784969047</v>
+        <v>4.56696826829867</v>
       </c>
       <c r="L3" t="n">
-        <v>2.16478916665764</v>
+        <v>4.508682009712</v>
       </c>
       <c r="M3" t="n">
-        <v>2.17286535719865</v>
+        <v>5.05170398532267</v>
       </c>
       <c r="N3" t="n">
-        <v>2.19792969281145</v>
+        <v>4.88591768026667</v>
       </c>
       <c r="O3" t="n">
-        <v>2.22962595826111</v>
+        <v>5.50042406870933</v>
       </c>
       <c r="P3" t="n">
-        <v>2.30132342918741</v>
+        <v>5.665169111376</v>
       </c>
       <c r="Q3" t="n">
-        <v>2.32485056153308</v>
+        <v>5.54685124291733</v>
       </c>
       <c r="R3" t="n">
-        <v>2.36697695891377</v>
+        <v>5.194334723936</v>
       </c>
       <c r="S3" t="n">
-        <v>2.41295919650284</v>
+        <v>5.48132627112533</v>
       </c>
       <c r="T3" t="n">
-        <v>2.38958961833115</v>
+        <v>4.80616361454933</v>
       </c>
       <c r="U3" t="n">
-        <v>2.39734350823087</v>
+        <v>4.97515829509867</v>
       </c>
       <c r="V3" t="n">
-        <v>2.42369399191491</v>
+        <v>5.86615657340267</v>
       </c>
       <c r="W3" t="n">
-        <v>2.48904102467887</v>
+        <v>5.33731686335467</v>
       </c>
       <c r="X3" t="n">
-        <v>2.51698737323723</v>
+        <v>5.06208077041067</v>
       </c>
       <c r="Y3" t="n">
-        <v>2.56126719613138</v>
+        <v>5.444890438976</v>
       </c>
       <c r="Z3" t="n">
-        <v>2.56549165462663</v>
+        <v>5.62006774946133</v>
       </c>
       <c r="AA3" t="n">
-        <v>2.58959347004699</v>
+        <v>6.04309861895467</v>
       </c>
       <c r="AB3" t="n">
-        <v>2.61391739193085</v>
+        <v>6.2484473756</v>
       </c>
       <c r="AC3" t="n">
-        <v>2.6256868631308</v>
+        <v>5.69877314173867</v>
       </c>
       <c r="AD3" t="n">
-        <v>2.62698499662995</v>
+        <v>5.573991504624</v>
       </c>
       <c r="AE3" t="n">
-        <v>2.65875327649005</v>
+        <v>5.69026309869867</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>6.6050388476</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" t="s">
         <v>39</v>
       </c>
-      <c r="B4" t="n">
+      <c r="C4" t="n">
         <v>8.17558268994896</v>
       </c>
-      <c r="C4" t="n">
+      <c r="D4" t="n">
         <v>8.12067446057568</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>8.12317937232918</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>8.1112387252679</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>8.16810972379053</v>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>8.28068280353069</v>
       </c>
-      <c r="H4" t="n">
+      <c r="I4" t="n">
         <v>8.37851843757582</v>
       </c>
-      <c r="I4" t="n">
+      <c r="J4" t="n">
         <v>8.37251836824657</v>
       </c>
-      <c r="J4" t="n">
+      <c r="K4" t="n">
         <v>8.28089621769761</v>
       </c>
-      <c r="K4" t="n">
+      <c r="L4" t="n">
         <v>8.31341871672003</v>
       </c>
-      <c r="L4" t="n">
+      <c r="M4" t="n">
         <v>8.43768841872268</v>
       </c>
-      <c r="M4" t="n">
+      <c r="N4" t="n">
         <v>8.45155015493985</v>
       </c>
-      <c r="N4" t="n">
+      <c r="O4" t="n">
         <v>8.44785213115087</v>
       </c>
-      <c r="O4" t="n">
+      <c r="P4" t="n">
         <v>8.71209103314128</v>
       </c>
-      <c r="P4" t="n">
+      <c r="Q4" t="n">
         <v>8.91054288223696</v>
       </c>
-      <c r="Q4" t="n">
+      <c r="R4" t="n">
         <v>9.09171059846931</v>
       </c>
-      <c r="R4" t="n">
+      <c r="S4" t="n">
         <v>9.2690085174304</v>
       </c>
-      <c r="S4" t="n">
+      <c r="T4" t="n">
         <v>9.35468547686209</v>
       </c>
-      <c r="T4" t="n">
+      <c r="U4" t="n">
         <v>9.5155069286025</v>
       </c>
-      <c r="U4" t="n">
+      <c r="V4" t="n">
         <v>9.49267164996975</v>
       </c>
-      <c r="V4" t="n">
+      <c r="W4" t="n">
         <v>9.66424928526536</v>
       </c>
-      <c r="W4" t="n">
+      <c r="X4" t="n">
         <v>9.86385217207488</v>
       </c>
-      <c r="X4" t="n">
+      <c r="Y4" t="n">
         <v>9.99916003902629</v>
       </c>
-      <c r="Y4" t="n">
+      <c r="Z4" t="n">
         <v>10.0557372142805</v>
       </c>
-      <c r="Z4" t="n">
+      <c r="AA4" t="n">
         <v>10.1368965268333</v>
       </c>
-      <c r="AA4" t="n">
+      <c r="AB4" t="n">
         <v>10.1894129760287</v>
       </c>
-      <c r="AB4" t="n">
+      <c r="AC4" t="n">
         <v>10.2315332243296</v>
       </c>
-      <c r="AC4" t="n">
+      <c r="AD4" t="n">
         <v>10.3727142481189</v>
       </c>
-      <c r="AD4" t="n">
+      <c r="AE4" t="n">
         <v>10.4542093297495</v>
       </c>
-      <c r="AE4" t="n">
+      <c r="AF4" t="n">
         <v>10.5651795494206</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5" t="n">
-        <v>4.979180807728</v>
+        <v>42</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
       </c>
       <c r="C5" t="n">
-        <v>4.93705854162133</v>
+        <v>2.00642716754084</v>
       </c>
       <c r="D5" t="n">
-        <v>4.94476376996267</v>
+        <v>1.99939597916104</v>
       </c>
       <c r="E5" t="n">
-        <v>4.95038710129067</v>
+        <v>2.01570991212078</v>
       </c>
       <c r="F5" t="n">
-        <v>4.92721480013867</v>
+        <v>2.01129632106231</v>
       </c>
       <c r="G5" t="n">
-        <v>4.89187336204267</v>
+        <v>2.05574953817727</v>
       </c>
       <c r="H5" t="n">
-        <v>4.829820287952</v>
+        <v>2.11970750819197</v>
       </c>
       <c r="I5" t="n">
-        <v>6.55340794822933</v>
+        <v>2.16758632501459</v>
       </c>
       <c r="J5" t="n">
-        <v>4.56696826829867</v>
+        <v>2.1574787499978</v>
       </c>
       <c r="K5" t="n">
-        <v>4.508682009712</v>
+        <v>2.14042841905745</v>
       </c>
       <c r="L5" t="n">
-        <v>5.05170398532267</v>
+        <v>2.14834784969047</v>
       </c>
       <c r="M5" t="n">
-        <v>4.88591768026667</v>
+        <v>2.16478916665764</v>
       </c>
       <c r="N5" t="n">
-        <v>5.50042406870933</v>
+        <v>2.17286535719865</v>
       </c>
       <c r="O5" t="n">
-        <v>5.665169111376</v>
+        <v>2.19792969281145</v>
       </c>
       <c r="P5" t="n">
-        <v>5.54685124291733</v>
+        <v>2.22962595826111</v>
       </c>
       <c r="Q5" t="n">
-        <v>5.194334723936</v>
+        <v>2.30132342918741</v>
       </c>
       <c r="R5" t="n">
-        <v>5.48132627112533</v>
+        <v>2.32485056153308</v>
       </c>
       <c r="S5" t="n">
-        <v>4.80616361454933</v>
+        <v>2.36697695891377</v>
       </c>
       <c r="T5" t="n">
-        <v>4.97515829509867</v>
+        <v>2.41295919650284</v>
       </c>
       <c r="U5" t="n">
-        <v>5.86615657340267</v>
+        <v>2.38958961833115</v>
       </c>
       <c r="V5" t="n">
-        <v>5.33731686335467</v>
+        <v>2.39734350823087</v>
       </c>
       <c r="W5" t="n">
-        <v>5.06208077041067</v>
+        <v>2.42369399191491</v>
       </c>
       <c r="X5" t="n">
-        <v>5.444890438976</v>
+        <v>2.48904102467887</v>
       </c>
       <c r="Y5" t="n">
-        <v>5.62006774946133</v>
+        <v>2.51698737323723</v>
       </c>
       <c r="Z5" t="n">
-        <v>6.04309861895467</v>
+        <v>2.56126719613138</v>
       </c>
       <c r="AA5" t="n">
-        <v>6.2484473756</v>
+        <v>2.56549165462663</v>
       </c>
       <c r="AB5" t="n">
-        <v>5.69877314173867</v>
+        <v>2.58959347004699</v>
       </c>
       <c r="AC5" t="n">
-        <v>5.573991504624</v>
+        <v>2.61391739193085</v>
       </c>
       <c r="AD5" t="n">
-        <v>5.69026309869867</v>
+        <v>2.6256868631308</v>
       </c>
       <c r="AE5" t="n">
-        <v>6.6050388476</v>
+        <v>2.62698499662995</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>2.65875327649005</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.381216423881282</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.396099605425283</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.403242312333865</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.415991162732946</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.449428755046009</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.498128786341533</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.531939552487414</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.566835583280444</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.59561157093514</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.61777226901104</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.655705087850153</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.660155956268442</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0.737170097917884</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0.767393658719658</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0.8480087680807</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0.908472287744949</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0.877785810766169</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0.879118168819757</v>
+      </c>
+      <c r="U6" t="n">
+        <v>0.855568648353471</v>
+      </c>
+      <c r="V6" t="n">
+        <v>0.877874049586454</v>
+      </c>
+      <c r="W6" t="n">
+        <v>0.942758172493304</v>
+      </c>
+      <c r="X6" t="n">
+        <v>0.998046611981724</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>1.05967117039715</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>1.11234348344948</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>1.19209320678856</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>1.15386683147162</v>
+      </c>
+      <c r="AC6" t="n">
+        <v>1.20861676001377</v>
+      </c>
+      <c r="AD6" t="n">
+        <v>1.27784706057641</v>
+      </c>
+      <c r="AE6" t="n">
+        <v>1.34470422904084</v>
+      </c>
+      <c r="AF6" t="n">
+        <v>1.35028402604853</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" t="n">
+        <v>38.2702896008102</v>
+      </c>
+      <c r="D7" t="n">
+        <v>38.3140340325882</v>
+      </c>
+      <c r="E7" t="n">
+        <v>38.2842158524957</v>
+      </c>
+      <c r="F7" t="n">
+        <v>38.3841160680714</v>
+      </c>
+      <c r="G7" t="n">
+        <v>38.7346637006567</v>
+      </c>
+      <c r="H7" t="n">
+        <v>39.5818103628589</v>
+      </c>
+      <c r="I7" t="n">
+        <v>40.1468184014891</v>
+      </c>
+      <c r="J7" t="n">
+        <v>42.3398585506587</v>
+      </c>
+      <c r="K7" t="n">
+        <v>40.4084308847629</v>
+      </c>
+      <c r="L7" t="n">
+        <v>40.5887678435164</v>
+      </c>
+      <c r="M7" t="n">
+        <v>42.1572047453664</v>
+      </c>
+      <c r="N7" t="n">
+        <v>42.3420780874897</v>
+      </c>
+      <c r="O7" t="n">
+        <v>43.4177950570983</v>
+      </c>
+      <c r="P7" t="n">
+        <v>45.1738065721724</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>46.699274497559</v>
+      </c>
+      <c r="R7" t="n">
+        <v>47.6893935016758</v>
+      </c>
+      <c r="S7" t="n">
+        <v>49.1956674593717</v>
+      </c>
+      <c r="T7" t="n">
+        <v>49.8589579856948</v>
+      </c>
+      <c r="U7" t="n">
+        <v>50.3573215840125</v>
+      </c>
+      <c r="V7" t="n">
+        <v>50.9143618335045</v>
+      </c>
+      <c r="W7" t="n">
+        <v>52.5487454496572</v>
+      </c>
+      <c r="X7" t="n">
+        <v>53.5987337616796</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>54.7260135482166</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>55.5202845694718</v>
+      </c>
+      <c r="AA7" t="n">
+        <v>56.308127703112</v>
+      </c>
+      <c r="AB7" t="n">
+        <v>56.5672688429137</v>
+      </c>
+      <c r="AC7" t="n">
+        <v>56.2184299790782</v>
+      </c>
+      <c r="AD7" t="n">
+        <v>56.7858329440775</v>
+      </c>
+      <c r="AE7" t="n">
+        <v>57.8323423240893</v>
+      </c>
+      <c r="AF7" t="n">
+        <v>59.0906248276123</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1.81823060093689</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1.82886443566439</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1.82378563885994</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1.83161622061741</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1.85073287068034</v>
+      </c>
+      <c r="H8" t="n">
+        <v>1.90331343222016</v>
+      </c>
+      <c r="I8" t="n">
+        <v>1.93911630387674</v>
+      </c>
+      <c r="J8" t="n">
+        <v>1.97516943207236</v>
+      </c>
+      <c r="K8" t="n">
+        <v>1.98596211270193</v>
+      </c>
+      <c r="L8" t="n">
+        <v>2.00004375987063</v>
+      </c>
+      <c r="M8" t="n">
+        <v>2.06778544694506</v>
+      </c>
+      <c r="N8" t="n">
+        <v>2.09372711510529</v>
+      </c>
+      <c r="O8" t="n">
+        <v>2.1227535253207</v>
+      </c>
+      <c r="P8" t="n">
+        <v>2.22396214485394</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>2.32740385401092</v>
+      </c>
+      <c r="R8" t="n">
+        <v>2.4136020263994</v>
+      </c>
+      <c r="S8" t="n">
+        <v>2.49604559209089</v>
+      </c>
+      <c r="T8" t="n">
+        <v>2.59248252231686</v>
+      </c>
+      <c r="U8" t="n">
+        <v>2.60971984749013</v>
+      </c>
+      <c r="V8" t="n">
+        <v>2.58242528418518</v>
+      </c>
+      <c r="W8" t="n">
+        <v>2.73445817093032</v>
+      </c>
+      <c r="X8" t="n">
+        <v>2.81485705460267</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>2.8564243621264</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>2.89366951409193</v>
+      </c>
+      <c r="AA8" t="n">
+        <v>2.90964381567271</v>
+      </c>
+      <c r="AB8" t="n">
+        <v>2.91087585518132</v>
+      </c>
+      <c r="AC8" t="n">
+        <v>2.91724715688522</v>
+      </c>
+      <c r="AD8" t="n">
+        <v>2.95484746141018</v>
+      </c>
+      <c r="AE8" t="n">
+        <v>3.01729445359763</v>
+      </c>
+      <c r="AF8" t="n">
+        <v>3.03290953024425</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" t="n">
+        <v>3.4854265654096</v>
+      </c>
+      <c r="D9" t="n">
+        <v>3.45594097913493</v>
+      </c>
+      <c r="E9" t="n">
+        <v>3.46133463897387</v>
+      </c>
+      <c r="F9" t="n">
+        <v>3.46527097090347</v>
+      </c>
+      <c r="G9" t="n">
+        <v>3.44905036009707</v>
+      </c>
+      <c r="H9" t="n">
+        <v>3.42431135342987</v>
+      </c>
+      <c r="I9" t="n">
+        <v>3.3808742015664</v>
+      </c>
+      <c r="J9" t="n">
+        <v>4.58738556376053</v>
+      </c>
+      <c r="K9" t="n">
+        <v>3.19687778780907</v>
+      </c>
+      <c r="L9" t="n">
+        <v>3.1560774067984</v>
+      </c>
+      <c r="M9" t="n">
+        <v>3.53619278972587</v>
+      </c>
+      <c r="N9" t="n">
+        <v>3.42014237618667</v>
+      </c>
+      <c r="O9" t="n">
+        <v>3.85029684809653</v>
+      </c>
+      <c r="P9" t="n">
+        <v>3.9656183779632</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>3.88279587004213</v>
+      </c>
+      <c r="R9" t="n">
+        <v>3.6360343067552</v>
+      </c>
+      <c r="S9" t="n">
+        <v>3.83692838978773</v>
+      </c>
+      <c r="T9" t="n">
+        <v>3.36431453018453</v>
+      </c>
+      <c r="U9" t="n">
+        <v>3.48261080656907</v>
+      </c>
+      <c r="V9" t="n">
+        <v>4.10630960138187</v>
+      </c>
+      <c r="W9" t="n">
+        <v>3.73612180434827</v>
+      </c>
+      <c r="X9" t="n">
+        <v>3.54345653928747</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>3.8114233072832</v>
+      </c>
+      <c r="Z9" t="n">
+        <v>3.93404742462293</v>
+      </c>
+      <c r="AA9" t="n">
+        <v>4.23016903326827</v>
+      </c>
+      <c r="AB9" t="n">
+        <v>4.37391316292</v>
+      </c>
+      <c r="AC9" t="n">
+        <v>3.98914119921707</v>
+      </c>
+      <c r="AD9" t="n">
+        <v>3.9017940532368</v>
+      </c>
+      <c r="AE9" t="n">
+        <v>3.98318416908907</v>
+      </c>
+      <c r="AF9" t="n">
+        <v>4.62352719332</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
         <v>41</v>
       </c>
-      <c r="B6" t="n">
-        <v>22.7278825117111</v>
-      </c>
-      <c r="C6" t="n">
-        <v>22.8608054458048</v>
-      </c>
-      <c r="D6" t="n">
-        <v>22.7973204857492</v>
-      </c>
-      <c r="E6" t="n">
-        <v>22.8952027577176</v>
-      </c>
-      <c r="F6" t="n">
-        <v>23.1341608835042</v>
-      </c>
-      <c r="G6" t="n">
-        <v>23.791417902752</v>
-      </c>
-      <c r="H6" t="n">
-        <v>24.2389537984593</v>
-      </c>
-      <c r="I6" t="n">
-        <v>24.6896179009045</v>
-      </c>
-      <c r="J6" t="n">
-        <v>24.8245264087741</v>
-      </c>
-      <c r="K6" t="n">
-        <v>25.0005469983828</v>
-      </c>
-      <c r="L6" t="n">
-        <v>25.8473180868132</v>
-      </c>
-      <c r="M6" t="n">
-        <v>26.1715889388161</v>
-      </c>
-      <c r="N6" t="n">
-        <v>26.5344190665088</v>
-      </c>
-      <c r="O6" t="n">
-        <v>27.7995268106743</v>
-      </c>
-      <c r="P6" t="n">
-        <v>29.0925481751366</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>30.1700253299925</v>
-      </c>
-      <c r="R6" t="n">
-        <v>31.2005699011361</v>
-      </c>
-      <c r="S6" t="n">
-        <v>32.4060315289608</v>
-      </c>
-      <c r="T6" t="n">
-        <v>32.6214980936267</v>
-      </c>
-      <c r="U6" t="n">
-        <v>32.2803160523147</v>
-      </c>
-      <c r="V6" t="n">
-        <v>34.180727136629</v>
-      </c>
-      <c r="W6" t="n">
-        <v>35.1857131825334</v>
-      </c>
-      <c r="X6" t="n">
-        <v>35.70530452658</v>
-      </c>
-      <c r="Y6" t="n">
-        <v>36.1708689261492</v>
-      </c>
-      <c r="Z6" t="n">
-        <v>36.3705476959089</v>
-      </c>
-      <c r="AA6" t="n">
-        <v>36.3859481897665</v>
-      </c>
-      <c r="AB6" t="n">
-        <v>36.4655894610653</v>
-      </c>
-      <c r="AC6" t="n">
-        <v>36.9355932676273</v>
-      </c>
-      <c r="AD6" t="n">
-        <v>37.7161806699703</v>
-      </c>
-      <c r="AE6" t="n">
-        <v>37.9113691280531</v>
+      <c r="B10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" t="n">
+        <v>2.45267480698469</v>
+      </c>
+      <c r="D10" t="n">
+        <v>2.4362023381727</v>
+      </c>
+      <c r="E10" t="n">
+        <v>2.43695381169875</v>
+      </c>
+      <c r="F10" t="n">
+        <v>2.43337161758037</v>
+      </c>
+      <c r="G10" t="n">
+        <v>2.45043291713716</v>
+      </c>
+      <c r="H10" t="n">
+        <v>2.48420484105921</v>
+      </c>
+      <c r="I10" t="n">
+        <v>2.51355553127275</v>
+      </c>
+      <c r="J10" t="n">
+        <v>2.51175551047397</v>
+      </c>
+      <c r="K10" t="n">
+        <v>2.48426886530928</v>
+      </c>
+      <c r="L10" t="n">
+        <v>2.49402561501601</v>
+      </c>
+      <c r="M10" t="n">
+        <v>2.5313065256168</v>
+      </c>
+      <c r="N10" t="n">
+        <v>2.53546504648195</v>
+      </c>
+      <c r="O10" t="n">
+        <v>2.53435563934526</v>
+      </c>
+      <c r="P10" t="n">
+        <v>2.61362730994238</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>2.67316286467109</v>
+      </c>
+      <c r="R10" t="n">
+        <v>2.72751317954079</v>
+      </c>
+      <c r="S10" t="n">
+        <v>2.78070255522912</v>
+      </c>
+      <c r="T10" t="n">
+        <v>2.80640564305863</v>
+      </c>
+      <c r="U10" t="n">
+        <v>2.85465207858075</v>
+      </c>
+      <c r="V10" t="n">
+        <v>2.84780149499092</v>
+      </c>
+      <c r="W10" t="n">
+        <v>2.89927478557961</v>
+      </c>
+      <c r="X10" t="n">
+        <v>2.95915565162246</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>2.99974801170789</v>
+      </c>
+      <c r="Z10" t="n">
+        <v>3.01672116428414</v>
+      </c>
+      <c r="AA10" t="n">
+        <v>3.04106895804998</v>
+      </c>
+      <c r="AB10" t="n">
+        <v>3.0568238928086</v>
+      </c>
+      <c r="AC10" t="n">
+        <v>3.06945996729888</v>
+      </c>
+      <c r="AD10" t="n">
+        <v>3.11181427443568</v>
+      </c>
+      <c r="AE10" t="n">
+        <v>3.13626279892485</v>
+      </c>
+      <c r="AF10" t="n">
+        <v>3.16955386482619</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1.20385630052451</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1.19963758749663</v>
+      </c>
+      <c r="E11" t="n">
+        <v>1.20942594727247</v>
+      </c>
+      <c r="F11" t="n">
+        <v>1.20677779263739</v>
+      </c>
+      <c r="G11" t="n">
+        <v>1.23344972290636</v>
+      </c>
+      <c r="H11" t="n">
+        <v>1.27182450491518</v>
+      </c>
+      <c r="I11" t="n">
+        <v>1.30055179500875</v>
+      </c>
+      <c r="J11" t="n">
+        <v>1.29448724999868</v>
+      </c>
+      <c r="K11" t="n">
+        <v>1.28425705143447</v>
+      </c>
+      <c r="L11" t="n">
+        <v>1.28900870981428</v>
+      </c>
+      <c r="M11" t="n">
+        <v>1.29887349999458</v>
+      </c>
+      <c r="N11" t="n">
+        <v>1.30371921431919</v>
+      </c>
+      <c r="O11" t="n">
+        <v>1.31875781568687</v>
+      </c>
+      <c r="P11" t="n">
+        <v>1.33777557495667</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>1.38079405751245</v>
+      </c>
+      <c r="R11" t="n">
+        <v>1.39491033691985</v>
+      </c>
+      <c r="S11" t="n">
+        <v>1.42018617534826</v>
+      </c>
+      <c r="T11" t="n">
+        <v>1.4477755179017</v>
+      </c>
+      <c r="U11" t="n">
+        <v>1.43375377099869</v>
+      </c>
+      <c r="V11" t="n">
+        <v>1.43840610493852</v>
+      </c>
+      <c r="W11" t="n">
+        <v>1.45421639514894</v>
+      </c>
+      <c r="X11" t="n">
+        <v>1.49342461480732</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>1.51019242394234</v>
+      </c>
+      <c r="Z11" t="n">
+        <v>1.53676031767883</v>
+      </c>
+      <c r="AA11" t="n">
+        <v>1.53929499277598</v>
+      </c>
+      <c r="AB11" t="n">
+        <v>1.5537560820282</v>
+      </c>
+      <c r="AC11" t="n">
+        <v>1.56835043515851</v>
+      </c>
+      <c r="AD11" t="n">
+        <v>1.57541211787848</v>
+      </c>
+      <c r="AE11" t="n">
+        <v>1.57619099797797</v>
+      </c>
+      <c r="AF11" t="n">
+        <v>1.59525196589403</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.114364927164385</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.118829881627585</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.120972693700159</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.124797348819884</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.134828626513803</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.14943863590246</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.159581865746224</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0.170050674984133</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.178683471280542</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0.185331680703312</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0.196711526355046</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0.198046786880533</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0.221151029375365</v>
+      </c>
+      <c r="P12" t="n">
+        <v>0.230218097615897</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>0.25440263042421</v>
+      </c>
+      <c r="R12" t="n">
+        <v>0.272541686323485</v>
+      </c>
+      <c r="S12" t="n">
+        <v>0.263335743229851</v>
+      </c>
+      <c r="T12" t="n">
+        <v>0.263735450645927</v>
+      </c>
+      <c r="U12" t="n">
+        <v>0.256670594506041</v>
+      </c>
+      <c r="V12" t="n">
+        <v>0.263362214875936</v>
+      </c>
+      <c r="W12" t="n">
+        <v>0.282827451747991</v>
+      </c>
+      <c r="X12" t="n">
+        <v>0.299413983594517</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>0.317901351119144</v>
+      </c>
+      <c r="Z12" t="n">
+        <v>0.333703045034844</v>
+      </c>
+      <c r="AA12" t="n">
+        <v>0.357627962036567</v>
+      </c>
+      <c r="AB12" t="n">
+        <v>0.346160049441487</v>
+      </c>
+      <c r="AC12" t="n">
+        <v>0.36258502800413</v>
+      </c>
+      <c r="AD12" t="n">
+        <v>0.383354118172923</v>
+      </c>
+      <c r="AE12" t="n">
+        <v>0.403411268712253</v>
+      </c>
+      <c r="AF12" t="n">
+        <v>0.405085207814559</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" t="n">
+        <v>4.78874972187329</v>
+      </c>
+      <c r="D13" t="n">
+        <v>4.76199599852022</v>
+      </c>
+      <c r="E13" t="n">
+        <v>4.76687748262761</v>
+      </c>
+      <c r="F13" t="n">
+        <v>4.77033597660961</v>
+      </c>
+      <c r="G13" t="n">
+        <v>4.7817736253358</v>
+      </c>
+      <c r="H13" t="n">
+        <v>4.8124477593054</v>
+      </c>
+      <c r="I13" t="n">
+        <v>4.81926811444904</v>
+      </c>
+      <c r="J13" t="n">
+        <v>5.74098691976037</v>
+      </c>
+      <c r="K13" t="n">
+        <v>4.69221790366641</v>
+      </c>
+      <c r="L13" t="n">
+        <v>4.67729138426356</v>
+      </c>
+      <c r="M13" t="n">
+        <v>4.99136019747386</v>
+      </c>
+      <c r="N13" t="n">
+        <v>4.92428232612889</v>
+      </c>
+      <c r="O13" t="n">
+        <v>5.2480336135198</v>
+      </c>
+      <c r="P13" t="n">
+        <v>5.4171790000036</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>5.4415094502138</v>
+      </c>
+      <c r="R13" t="n">
+        <v>5.33906379294523</v>
+      </c>
+      <c r="S13" t="n">
+        <v>5.54714739781862</v>
+      </c>
+      <c r="T13" t="n">
+        <v>5.29916039180581</v>
+      </c>
+      <c r="U13" t="n">
+        <v>5.4046076520038</v>
+      </c>
+      <c r="V13" t="n">
+        <v>5.81197419338912</v>
+      </c>
+      <c r="W13" t="n">
+        <v>5.66007054719056</v>
+      </c>
+      <c r="X13" t="n">
+        <v>5.61747919158399</v>
+      </c>
+      <c r="Y13" t="n">
+        <v>5.83663758717058</v>
+      </c>
+      <c r="Z13" t="n">
+        <v>5.95177695946892</v>
+      </c>
+      <c r="AA13" t="n">
+        <v>6.1729882897779</v>
+      </c>
+      <c r="AB13" t="n">
+        <v>6.28350790999398</v>
+      </c>
+      <c r="AC13" t="n">
+        <v>6.03625330503045</v>
+      </c>
+      <c r="AD13" t="n">
+        <v>6.02224145594781</v>
+      </c>
+      <c r="AE13" t="n">
+        <v>6.11989256460794</v>
+      </c>
+      <c r="AF13" t="n">
+        <v>6.58259359890381</v>
       </c>
     </row>
   </sheetData>
@@ -1161,13 +1938,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2">
@@ -1246,22 +2023,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B1" t="s">
         <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="F1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2">
@@ -1269,7 +2046,7 @@
         <v>1990</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C2" t="n">
         <v>0.381216423881282</v>
@@ -1289,7 +2066,7 @@
         <v>1990</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C3" t="n">
         <v>2.00642716754084</v>
@@ -1309,7 +2086,7 @@
         <v>1990</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C4" t="n">
         <v>8.17558268994896</v>
@@ -1349,7 +2126,7 @@
         <v>1990</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C6" t="n">
         <v>22.7278825117111</v>
@@ -1369,7 +2146,7 @@
         <v>2000</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C7" t="n">
         <v>0.655705087850153</v>
@@ -1389,7 +2166,7 @@
         <v>2000</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C8" t="n">
         <v>2.16478916665764</v>
@@ -1409,7 +2186,7 @@
         <v>2000</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C9" t="n">
         <v>8.43768841872268</v>
@@ -1449,7 +2226,7 @@
         <v>2000</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C11" t="n">
         <v>25.8473180868132</v>
@@ -1469,7 +2246,7 @@
         <v>2010</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C12" t="n">
         <v>0.942758172493304</v>
@@ -1489,7 +2266,7 @@
         <v>2010</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C13" t="n">
         <v>2.42369399191491</v>
@@ -1509,7 +2286,7 @@
         <v>2010</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C14" t="n">
         <v>9.66424928526536</v>
@@ -1549,7 +2326,7 @@
         <v>2010</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C16" t="n">
         <v>34.180727136629</v>
@@ -1569,7 +2346,7 @@
         <v>2019</v>
       </c>
       <c r="B17" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C17" t="n">
         <v>1.35028402604853</v>
@@ -1589,7 +2366,7 @@
         <v>2019</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C18" t="n">
         <v>2.65875327649005</v>
@@ -1609,7 +2386,7 @@
         <v>2019</v>
       </c>
       <c r="B19" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C19" t="n">
         <v>10.5651795494206</v>
@@ -1649,7 +2426,7 @@
         <v>2019</v>
       </c>
       <c r="B21" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C21" t="n">
         <v>37.9113691280531</v>
@@ -1680,40 +2457,40 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B1" t="s">
         <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="F1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="H1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="I1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="J1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="K1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="L1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2">
@@ -1721,10 +2498,10 @@
         <v>2019</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D2" t="n">
         <v>37.9113691280531</v>
@@ -1762,7 +2539,7 @@
         <v>40</v>
       </c>
       <c r="C3" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D3" t="n">
         <v>6.6050388476</v>
@@ -1797,10 +2574,10 @@
         <v>2019</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C4" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D4" t="n">
         <v>7.96355304750256</v>
@@ -1835,10 +2612,10 @@
         <v>2019</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C5" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D5" t="n">
         <v>3.01909712714988</v>
@@ -1873,10 +2650,10 @@
         <v>2019</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C6" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D6" t="n">
         <v>1.09585188334429</v>
@@ -1911,10 +2688,10 @@
         <v>2019</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D7" t="n">
         <v>37.9113691280531</v>
@@ -1952,7 +2729,7 @@
         <v>40</v>
       </c>
       <c r="C8" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D8" t="n">
         <v>6.6050388476</v>
@@ -1987,10 +2764,10 @@
         <v>2019</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C9" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D9" t="n">
         <v>10.851160466577</v>
@@ -2025,10 +2802,10 @@
         <v>2019</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C10" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D10" t="n">
         <v>2.58084109256361</v>
@@ -2063,10 +2840,10 @@
         <v>2019</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D11" t="n">
         <v>1.16730049866546</v>
@@ -2101,10 +2878,10 @@
         <v>2019</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D12" t="n">
         <v>37.9113691280531</v>
@@ -2142,7 +2919,7 @@
         <v>40</v>
       </c>
       <c r="C13" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D13" t="n">
         <v>6.6050388476</v>
@@ -2177,10 +2954,10 @@
         <v>2019</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C14" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D14" t="n">
         <v>13.126461337292</v>
@@ -2215,10 +2992,10 @@
         <v>2019</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C15" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D15" t="n">
         <v>2.90222885126021</v>
@@ -2253,10 +3030,10 @@
         <v>2019</v>
       </c>
       <c r="B16" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C16" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D16" t="n">
         <v>1.34789543653044</v>
@@ -2291,10 +3068,10 @@
         <v>2019</v>
       </c>
       <c r="B17" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C17" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D17" t="n">
         <v>37.9113691280531</v>
@@ -2332,7 +3109,7 @@
         <v>40</v>
       </c>
       <c r="C18" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D18" t="n">
         <v>6.6050388476</v>
@@ -2367,10 +3144,10 @@
         <v>2019</v>
       </c>
       <c r="B19" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C19" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D19" t="n">
         <v>10.5651795494206</v>
@@ -2405,10 +3182,10 @@
         <v>2019</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C20" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D20" t="n">
         <v>2.65875327649005</v>
@@ -2443,10 +3220,10 @@
         <v>2019</v>
       </c>
       <c r="B21" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C21" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D21" t="n">
         <v>1.35028402604853</v>
@@ -2492,19 +3269,19 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B1" t="s">
         <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2">
@@ -2512,7 +3289,7 @@
         <v>1990</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
@@ -2529,7 +3306,7 @@
         <v>1990</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
@@ -2546,7 +3323,7 @@
         <v>1990</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C4" t="n">
         <v>1</v>
@@ -2563,7 +3340,7 @@
         <v>1991</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C5" t="n">
         <v>1.00584845218314</v>
@@ -2580,7 +3357,7 @@
         <v>1991</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C6" t="n">
         <v>0.993783699609292</v>
@@ -2597,7 +3374,7 @@
         <v>1991</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C7" t="n">
         <v>0.996495667276865</v>
@@ -2614,7 +3391,7 @@
         <v>1992</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C8" t="n">
         <v>1.00305518888538</v>
@@ -2631,7 +3408,7 @@
         <v>1992</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C9" t="n">
         <v>0.993938154849664</v>
@@ -2648,7 +3425,7 @@
         <v>1992</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C10" t="n">
         <v>1.00462650462977</v>
@@ -2665,7 +3442,7 @@
         <v>1993</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C11" t="n">
         <v>1.00736189330089</v>
@@ -2682,7 +3459,7 @@
         <v>1993</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C12" t="n">
         <v>0.992318119354956</v>
@@ -2699,7 +3476,7 @@
         <v>1993</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C13" t="n">
         <v>1.002426778106</v>
@@ -2716,7 +3493,7 @@
         <v>1994</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C14" t="n">
         <v>1.01787576874281</v>
@@ -2733,7 +3510,7 @@
         <v>1994</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C15" t="n">
         <v>0.998984191401705</v>
@@ -2750,7 +3527,7 @@
         <v>1994</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C16" t="n">
         <v>1.02458218839654</v>
@@ -2767,7 +3544,7 @@
         <v>1995</v>
       </c>
       <c r="B17" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C17" t="n">
         <v>1.04679430169057</v>
@@ -2784,7 +3561,7 @@
         <v>1995</v>
       </c>
       <c r="B18" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C18" t="n">
         <v>1.01220047730783</v>
@@ -2801,7 +3578,7 @@
         <v>1995</v>
       </c>
       <c r="B19" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C19" t="n">
         <v>1.05645873544962</v>
@@ -2818,7 +3595,7 @@
         <v>1996</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C20" t="n">
         <v>1.06648535278064</v>
@@ -2835,7 +3612,7 @@
         <v>1996</v>
       </c>
       <c r="B21" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C21" t="n">
         <v>1.02318768162499</v>
@@ -2852,7 +3629,7 @@
         <v>1996</v>
       </c>
       <c r="B22" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C22" t="n">
         <v>1.08032145899981</v>
@@ -2869,7 +3646,7 @@
         <v>1997</v>
       </c>
       <c r="B23" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C23" t="n">
         <v>1.0863140412743</v>
@@ -2886,7 +3663,7 @@
         <v>1997</v>
       </c>
       <c r="B24" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C24" t="n">
         <v>1.02222602850794</v>
@@ -2903,7 +3680,7 @@
         <v>1997</v>
       </c>
       <c r="B25" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C25" t="n">
         <v>1.07528386023705</v>
@@ -2920,7 +3697,7 @@
         <v>1998</v>
       </c>
       <c r="B26" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C26" t="n">
         <v>1.09224985635959</v>
@@ -2937,7 +3714,7 @@
         <v>1998</v>
       </c>
       <c r="B27" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C27" t="n">
         <v>1.01150370886277</v>
@@ -2954,7 +3731,7 @@
         <v>1998</v>
       </c>
       <c r="B28" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C28" t="n">
         <v>1.06678600334187</v>
@@ -2971,7 +3748,7 @@
         <v>1999</v>
       </c>
       <c r="B29" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C29" t="n">
         <v>1.09999455450813</v>
@@ -2988,7 +3765,7 @@
         <v>1999</v>
       </c>
       <c r="B30" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C30" t="n">
         <v>1.01568845821745</v>
@@ -3005,7 +3782,7 @@
         <v>1999</v>
       </c>
       <c r="B31" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C31" t="n">
         <v>1.07073303454298</v>
@@ -3022,7 +3799,7 @@
         <v>2000</v>
       </c>
       <c r="B32" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C32" t="n">
         <v>1.13725148277648</v>
@@ -3039,7 +3816,7 @@
         <v>2000</v>
       </c>
       <c r="B33" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C33" t="n">
         <v>1.02993298583582</v>
@@ -3056,7 +3833,7 @@
         <v>2000</v>
       </c>
       <c r="B34" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C34" t="n">
         <v>1.07892735987566</v>
@@ -3073,7 +3850,7 @@
         <v>2001</v>
       </c>
       <c r="B35" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C35" t="n">
         <v>1.1515190174593</v>
@@ -3090,7 +3867,7 @@
         <v>2001</v>
       </c>
       <c r="B36" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C36" t="n">
         <v>1.03146432129483</v>
@@ -3107,7 +3884,7 @@
         <v>2001</v>
       </c>
       <c r="B37" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C37" t="n">
         <v>1.08295251995705</v>
@@ -3124,7 +3901,7 @@
         <v>2002</v>
       </c>
       <c r="B38" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C38" t="n">
         <v>1.16748311475282</v>
@@ -3141,7 +3918,7 @@
         <v>2002</v>
       </c>
       <c r="B39" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C39" t="n">
         <v>1.03155894996811</v>
@@ -3158,7 +3935,7 @@
         <v>2002</v>
       </c>
       <c r="B40" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C40" t="n">
         <v>1.09544454359902</v>
@@ -3175,7 +3952,7 @@
         <v>2003</v>
       </c>
       <c r="B41" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C41" t="n">
         <v>1.2231463620225</v>
@@ -3192,7 +3969,7 @@
         <v>2003</v>
       </c>
       <c r="B42" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C42" t="n">
         <v>1.06252347807712</v>
@@ -3209,7 +3986,7 @@
         <v>2003</v>
       </c>
       <c r="B43" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C43" t="n">
         <v>1.11124191016304</v>
@@ -3226,7 +4003,7 @@
         <v>2004</v>
       </c>
       <c r="B44" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C44" t="n">
         <v>1.2800377756329</v>
@@ -3243,7 +4020,7 @@
         <v>2004</v>
       </c>
       <c r="B45" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C45" t="n">
         <v>1.0864684888597</v>
@@ -3260,7 +4037,7 @@
         <v>2004</v>
       </c>
       <c r="B46" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C46" t="n">
         <v>1.14697581174003</v>
@@ -3277,7 +4054,7 @@
         <v>2005</v>
       </c>
       <c r="B47" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C47" t="n">
         <v>1.32744549847293</v>
@@ -3294,7 +4071,7 @@
         <v>2005</v>
       </c>
       <c r="B48" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C48" t="n">
         <v>1.10804979865503</v>
@@ -3311,7 +4088,7 @@
         <v>2005</v>
       </c>
       <c r="B49" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C49" t="n">
         <v>1.15870169580215</v>
@@ -3328,7 +4105,7 @@
         <v>2006</v>
       </c>
       <c r="B50" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C50" t="n">
         <v>1.37278824303404</v>
@@ -3345,7 +4122,7 @@
         <v>2006</v>
       </c>
       <c r="B51" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C51" t="n">
         <v>1.12939803791512</v>
@@ -3362,7 +4139,7 @@
         <v>2006</v>
       </c>
       <c r="B52" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C52" t="n">
         <v>1.17969742296444</v>
@@ -3379,7 +4156,7 @@
         <v>2007</v>
       </c>
       <c r="B53" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C53" t="n">
         <v>1.42582713159762</v>
@@ -3396,7 +4173,7 @@
         <v>2007</v>
       </c>
       <c r="B54" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C54" t="n">
         <v>1.14010736873668</v>
@@ -3413,7 +4190,7 @@
         <v>2007</v>
       </c>
       <c r="B55" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C55" t="n">
         <v>1.20261489454425</v>
@@ -3430,7 +4207,7 @@
         <v>2008</v>
       </c>
       <c r="B56" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C56" t="n">
         <v>1.43530740608227</v>
@@ -3447,7 +4224,7 @@
         <v>2008</v>
       </c>
       <c r="B57" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C57" t="n">
         <v>1.15952030139005</v>
@@ -3464,7 +4241,7 @@
         <v>2008</v>
       </c>
       <c r="B58" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C58" t="n">
         <v>1.19096753522328</v>
@@ -3481,7 +4258,7 @@
         <v>2009</v>
       </c>
       <c r="B59" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C59" t="n">
         <v>1.42029579903369</v>
@@ -3498,7 +4275,7 @@
         <v>2009</v>
       </c>
       <c r="B60" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C60" t="n">
         <v>1.15718071287271</v>
@@ -3515,7 +4292,7 @@
         <v>2009</v>
       </c>
       <c r="B61" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C61" t="n">
         <v>1.1948320611952</v>
@@ -3532,7 +4309,7 @@
         <v>2010</v>
       </c>
       <c r="B62" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C62" t="n">
         <v>1.50391164328733</v>
@@ -3549,7 +4326,7 @@
         <v>2010</v>
       </c>
       <c r="B63" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C63" t="n">
         <v>1.17742061880188</v>
@@ -3566,7 +4343,7 @@
         <v>2010</v>
       </c>
       <c r="B64" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C64" t="n">
         <v>1.20796509892033</v>
@@ -3583,7 +4360,7 @@
         <v>2011</v>
       </c>
       <c r="B65" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C65" t="n">
         <v>1.54812984291005</v>
@@ -3600,7 +4377,7 @@
         <v>2011</v>
       </c>
       <c r="B66" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C66" t="n">
         <v>1.2008684644021</v>
@@ -3617,7 +4394,7 @@
         <v>2011</v>
       </c>
       <c r="B67" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C67" t="n">
         <v>1.24053395256282</v>
@@ -3634,7 +4411,7 @@
         <v>2012</v>
       </c>
       <c r="B68" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C68" t="n">
         <v>1.5709912486648</v>
@@ -3651,7 +4428,7 @@
         <v>2012</v>
       </c>
       <c r="B69" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C69" t="n">
         <v>1.2171315877926</v>
@@ -3668,7 +4445,7 @@
         <v>2012</v>
       </c>
       <c r="B70" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C70" t="n">
         <v>1.25446236671633</v>
@@ -3685,7 +4462,7 @@
         <v>2013</v>
       </c>
       <c r="B71" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C71" t="n">
         <v>1.59147553264195</v>
@@ -3702,7 +4479,7 @@
         <v>2013</v>
       </c>
       <c r="B72" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C72" t="n">
         <v>1.22441706438054</v>
@@ -3719,7 +4496,7 @@
         <v>2013</v>
       </c>
       <c r="B73" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C73" t="n">
         <v>1.27653135761243</v>
@@ -3736,7 +4513,7 @@
         <v>2014</v>
       </c>
       <c r="B74" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C74" t="n">
         <v>1.60026116278839</v>
@@ -3753,7 +4530,7 @@
         <v>2014</v>
       </c>
       <c r="B75" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C75" t="n">
         <v>1.23426462055135</v>
@@ -3770,7 +4547,7 @@
         <v>2014</v>
       </c>
       <c r="B76" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C76" t="n">
         <v>1.2786368207778</v>
@@ -3787,7 +4564,7 @@
         <v>2015</v>
       </c>
       <c r="B77" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C77" t="n">
         <v>1.60093876633767</v>
@@ -3804,7 +4581,7 @@
         <v>2015</v>
       </c>
       <c r="B78" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C78" t="n">
         <v>1.24100081987417</v>
@@ -3821,7 +4598,7 @@
         <v>2015</v>
       </c>
       <c r="B79" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C79" t="n">
         <v>1.29064912593907</v>
@@ -3838,7 +4615,7 @@
         <v>2016</v>
       </c>
       <c r="B80" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C80" t="n">
         <v>1.60444288825743</v>
@@ -3855,7 +4632,7 @@
         <v>2016</v>
       </c>
       <c r="B81" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C81" t="n">
         <v>1.24662422750051</v>
@@ -3872,7 +4649,7 @@
         <v>2016</v>
       </c>
       <c r="B82" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C82" t="n">
         <v>1.30277212859641</v>
@@ -3889,7 +4666,7 @@
         <v>2017</v>
       </c>
       <c r="B83" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C83" t="n">
         <v>1.62512250090149</v>
@@ -3906,7 +4683,7 @@
         <v>2017</v>
       </c>
       <c r="B84" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C84" t="n">
         <v>1.26356091988598</v>
@@ -3923,7 +4700,7 @@
         <v>2017</v>
       </c>
       <c r="B85" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C85" t="n">
         <v>1.30863801368327</v>
@@ -3940,7 +4717,7 @@
         <v>2018</v>
       </c>
       <c r="B86" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C86" t="n">
         <v>1.65946742511257</v>
@@ -3957,7 +4734,7 @@
         <v>2018</v>
       </c>
       <c r="B87" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C87" t="n">
         <v>1.27358087495601</v>
@@ -3974,7 +4751,7 @@
         <v>2018</v>
       </c>
       <c r="B88" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C88" t="n">
         <v>1.30928500128399</v>
@@ -3991,7 +4768,7 @@
         <v>2019</v>
       </c>
       <c r="B89" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C89" t="n">
         <v>1.66805548684609</v>
@@ -4008,7 +4785,7 @@
         <v>2019</v>
       </c>
       <c r="B90" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C90" t="n">
         <v>1.28683030915669</v>
@@ -4025,7 +4802,7 @@
         <v>2019</v>
       </c>
       <c r="B91" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C91" t="n">
         <v>1.32511825971173</v>
@@ -4552,7 +5329,7 @@
         <v>1990</v>
       </c>
       <c r="B122" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C122" t="n">
         <v>1</v>
@@ -4569,7 +5346,7 @@
         <v>1991</v>
       </c>
       <c r="B123" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C123" t="n">
         <v>1.03904129153847</v>
@@ -4586,7 +5363,7 @@
         <v>1992</v>
       </c>
       <c r="B124" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C124" t="n">
         <v>1.0577779105851</v>
@@ -4603,7 +5380,7 @@
         <v>1993</v>
       </c>
       <c r="B125" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C125" t="n">
         <v>1.09122046342498</v>
@@ -4620,7 +5397,7 @@
         <v>1994</v>
       </c>
       <c r="B126" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C126" t="n">
         <v>1.17893334833331</v>
@@ -4637,7 +5414,7 @@
         <v>1995</v>
       </c>
       <c r="B127" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C127" t="n">
         <v>1.30668238600512</v>
@@ -4654,7 +5431,7 @@
         <v>1996</v>
       </c>
       <c r="B128" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C128" t="n">
         <v>1.39537417373463</v>
@@ -4671,7 +5448,7 @@
         <v>1997</v>
       </c>
       <c r="B129" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C129" t="n">
         <v>1.48691280797747</v>
@@ -4688,7 +5465,7 @@
         <v>1998</v>
       </c>
       <c r="B130" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C130" t="n">
         <v>1.56239745620358</v>
@@ -4705,7 +5482,7 @@
         <v>1999</v>
       </c>
       <c r="B131" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C131" t="n">
         <v>1.62052899694434</v>
@@ -4722,7 +5499,7 @@
         <v>2000</v>
       </c>
       <c r="B132" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C132" t="n">
         <v>1.72003367843971</v>
@@ -4739,7 +5516,7 @@
         <v>2001</v>
       </c>
       <c r="B133" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C133" t="n">
         <v>1.73170911564405</v>
@@ -4756,7 +5533,7 @@
         <v>2002</v>
       </c>
       <c r="B134" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C134" t="n">
         <v>1.93373121339456</v>
@@ -4773,7 +5550,7 @@
         <v>2003</v>
       </c>
       <c r="B135" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C135" t="n">
         <v>2.01301310921126</v>
@@ -4790,7 +5567,7 @@
         <v>2004</v>
       </c>
       <c r="B136" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C136" t="n">
         <v>2.22448120006704</v>
@@ -4807,7 +5584,7 @@
         <v>2005</v>
       </c>
       <c r="B137" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C137" t="n">
         <v>2.38308800679549</v>
@@ -4824,7 +5601,7 @@
         <v>2006</v>
       </c>
       <c r="B138" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C138" t="n">
         <v>2.3025917976701</v>
@@ -4841,7 +5618,7 @@
         <v>2007</v>
       </c>
       <c r="B139" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C139" t="n">
         <v>2.30608681511983</v>
@@ -4858,7 +5635,7 @@
         <v>2008</v>
       </c>
       <c r="B140" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C140" t="n">
         <v>2.24431214070649</v>
@@ -4875,7 +5652,7 @@
         <v>2009</v>
       </c>
       <c r="B141" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C141" t="n">
         <v>2.302823264141</v>
@@ -4892,7 +5669,7 @@
         <v>2010</v>
       </c>
       <c r="B142" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C142" t="n">
         <v>2.47302611701456</v>
@@ -4909,7 +5686,7 @@
         <v>2011</v>
       </c>
       <c r="B143" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C143" t="n">
         <v>2.61805774740842</v>
@@ -4926,7 +5703,7 @@
         <v>2012</v>
       </c>
       <c r="B144" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C144" t="n">
         <v>2.77971016990378</v>
@@ -4943,7 +5720,7 @@
         <v>2013</v>
       </c>
       <c r="B145" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C145" t="n">
         <v>2.91787922494096</v>
@@ -4960,7 +5737,7 @@
         <v>2014</v>
       </c>
       <c r="B146" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C146" t="n">
         <v>3.12707725089987</v>
@@ -4977,7 +5754,7 @@
         <v>2015</v>
       </c>
       <c r="B147" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C147" t="n">
         <v>3.02680251738304</v>
@@ -4994,7 +5771,7 @@
         <v>2016</v>
       </c>
       <c r="B148" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C148" t="n">
         <v>3.17042153564232</v>
@@ -5011,7 +5788,7 @@
         <v>2017</v>
       </c>
       <c r="B149" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C149" t="n">
         <v>3.35202520281329</v>
@@ -5028,7 +5805,7 @@
         <v>2018</v>
       </c>
       <c r="B150" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C150" t="n">
         <v>3.52740371296178</v>
@@ -5045,7 +5822,7 @@
         <v>2019</v>
       </c>
       <c r="B151" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C151" t="n">
         <v>3.54204053513978</v>
@@ -5055,6 +5832,112 @@
       </c>
       <c r="E151" t="n">
         <v>2.47942837459785</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G4" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>